<commit_message>
Update ICM20948 in nav hardware sheet
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/Avionics/nav-hardware-compare.xlsx
+++ b/docs/Avionics/nav-hardware-compare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARC\Research\docs\Avionics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E913D0-3474-462C-8DEB-435D28F2E44B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D4B60B-87B4-410B-9B5F-5ACE6708A4F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{45348F4D-BE45-4D91-992A-D063F65F5299}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="139">
   <si>
     <t>Metric</t>
   </si>
@@ -443,6 +443,12 @@
   </si>
   <si>
     <t>1.2-3.6 V</t>
+  </si>
+  <si>
+    <t>+-4900 microT</t>
+  </si>
+  <si>
+    <t>+-0.15 microT/LSB</t>
   </si>
 </sst>
 </file>
@@ -836,10 +842,10 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1188,6 +1194,9 @@
       <c r="A18" t="s">
         <v>65</v>
       </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
       <c r="I18" t="s">
         <v>35</v>
       </c>
@@ -1329,6 +1338,9 @@
       <c r="E24" t="s">
         <v>44</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="H24" t="s">
         <v>44</v>
       </c>
@@ -1351,6 +1363,9 @@
       </c>
       <c r="E25" t="s">
         <v>44</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="H25" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Add sensor data rates where known
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/Avionics/nav-hardware-compare.xlsx
+++ b/docs/Avionics/nav-hardware-compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARC\Research\docs\Avionics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D4B60B-87B4-410B-9B5F-5ACE6708A4F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE36DB2-1909-4383-8700-F480FB9B74E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{45348F4D-BE45-4D91-992A-D063F65F5299}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="151">
   <si>
     <t>Metric</t>
   </si>
@@ -449,6 +449,42 @@
   </si>
   <si>
     <t>+-0.15 microT/LSB</t>
+  </si>
+  <si>
+    <t>1000 LSB/g</t>
+  </si>
+  <si>
+    <t>16 LSB/deg/sec</t>
+  </si>
+  <si>
+    <t>Gyroscope output rate</t>
+  </si>
+  <si>
+    <t>8 kHz</t>
+  </si>
+  <si>
+    <t>Accelerometer output rate</t>
+  </si>
+  <si>
+    <t>1 kHz</t>
+  </si>
+  <si>
+    <t>9 kHz</t>
+  </si>
+  <si>
+    <t>4.5 kHz</t>
+  </si>
+  <si>
+    <t>Magnetometer output rate</t>
+  </si>
+  <si>
+    <t>100 Hz</t>
+  </si>
+  <si>
+    <t>523 Hz</t>
+  </si>
+  <si>
+    <t>30 Hz</t>
   </si>
 </sst>
 </file>
@@ -508,8 +544,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{770D4A71-5264-45AD-AC73-94F1A8371A49}" name="Table1" displayName="Table1" ref="A1:I25">
-  <autoFilter ref="A1:I25" xr:uid="{61742C8D-EB7E-430F-87EF-F491699C5324}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{770D4A71-5264-45AD-AC73-94F1A8371A49}" name="Table1" displayName="Table1" ref="A1:I28">
+  <autoFilter ref="A1:I28" xr:uid="{61742C8D-EB7E-430F-87EF-F491699C5324}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E4CD3989-8FA0-4468-A88B-C7C27B0C2CB8}" name="Metric" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{3AB6C83F-F853-460D-A1F7-457B3CBB579B}" name="ICM-20601"/>
@@ -839,13 +875,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1050,11 +1086,20 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="E9">
+        <v>5.25</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>15</v>
       </c>
+      <c r="G10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I10">
+        <v>12.07</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
@@ -1232,145 +1277,195 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" t="s">
-        <v>131</v>
+        <v>143</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>132</v>
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" t="s">
+        <v>131</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" t="s">
-        <v>133</v>
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I22" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" t="s">
+        <v>133</v>
+      </c>
+      <c r="I23" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H24" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>67</v>
+        <v>142</v>
+      </c>
+      <c r="G24" t="s">
+        <v>145</v>
+      </c>
+      <c r="I24" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>147</v>
+      </c>
+      <c r="G26" t="s">
+        <v>148</v>
+      </c>
+      <c r="I26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>44</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>44</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E28" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H28" t="s">
         <v>44</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I28" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor updates to BNO055 info
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/Avionics/nav-hardware-compare.xlsx
+++ b/docs/Avionics/nav-hardware-compare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARC\Research\docs\Avionics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE36DB2-1909-4383-8700-F480FB9B74E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4019ED2-CA5E-458C-9F45-938EE765EDC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{45348F4D-BE45-4D91-992A-D063F65F5299}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IMU" sheetId="1" r:id="rId1"/>
     <sheet name="GPS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="151">
   <si>
     <t>Metric</t>
   </si>
@@ -244,9 +244,6 @@
     <t>Self-test?</t>
   </si>
   <si>
-    <t>POST, BIST</t>
-  </si>
-  <si>
     <t>NEO-M8Q-01A</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>30 Hz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -984,7 +984,7 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I4" t="s">
         <v>61</v>
@@ -1042,7 +1042,7 @@
         <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I6" t="s">
         <v>63</v>
@@ -1076,7 +1076,7 @@
         <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I8" t="s">
         <v>58</v>
@@ -1097,14 +1097,17 @@
       <c r="G10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I10">
-        <v>12.07</v>
+      <c r="I10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>16</v>
       </c>
+      <c r="I11">
+        <v>34.950000000000003</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
@@ -1139,13 +1142,16 @@
       <c r="A13" t="s">
         <v>18</v>
       </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1269,7 +1275,7 @@
         <v>42</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>42</v>
@@ -1277,21 +1283,21 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1317,10 +1323,10 @@
         <v>43</v>
       </c>
       <c r="H21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1346,7 +1352,7 @@
         <v>51</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I22" t="s">
         <v>66</v>
@@ -1372,24 +1378,24 @@
         <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" t="s">
         <v>141</v>
       </c>
-      <c r="E24" t="s">
-        <v>142</v>
-      </c>
       <c r="G24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1408,13 +1414,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" t="s">
         <v>147</v>
       </c>
-      <c r="G26" t="s">
-        <v>148</v>
-      </c>
       <c r="I26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1434,7 +1440,7 @@
         <v>44</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H27" t="s">
         <v>44</v>
@@ -1460,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H28" t="s">
         <v>44</v>
@@ -1482,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50BCB51-82B5-48D2-BD5C-171740C85E68}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1499,16 +1505,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1516,16 +1522,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1533,13 +1539,13 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1547,13 +1553,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1561,13 +1567,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1585,27 +1591,27 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1623,13 +1629,13 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1647,7 +1653,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
@@ -1655,12 +1661,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -1674,7 +1680,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -1688,35 +1694,35 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21">
         <v>72</v>
@@ -1730,156 +1736,156 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" t="s">
         <v>120</v>
-      </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
         <v>92</v>
       </c>
-      <c r="B23" t="s">
-        <v>93</v>
-      </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add LEA M8S GPS data
Also noticed that the datasheets include a dynamic force limit

Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/Avionics/nav-hardware-compare.xlsx
+++ b/docs/Avionics/nav-hardware-compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARC\Research\docs\Avionics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4019ED2-CA5E-458C-9F45-938EE765EDC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E1FCC7-CE84-4BD0-AF01-F3CF62B9CBF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{45348F4D-BE45-4D91-992A-D063F65F5299}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{45348F4D-BE45-4D91-992A-D063F65F5299}"/>
   </bookViews>
   <sheets>
     <sheet name="IMU" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="159">
   <si>
     <t>Metric</t>
   </si>
@@ -485,6 +485,30 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>UART, USB, DDC</t>
+  </si>
+  <si>
+    <t>Limit: dynamics</t>
+  </si>
+  <si>
+    <t>&lt;= 4 g</t>
+  </si>
+  <si>
+    <t>22.4 mm</t>
+  </si>
+  <si>
+    <t>17 mm</t>
+  </si>
+  <si>
+    <t>2.1 gram</t>
+  </si>
+  <si>
+    <t>0.6 gram</t>
+  </si>
+  <si>
+    <t>1.6 gram</t>
   </si>
 </sst>
 </file>
@@ -562,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{04702736-6AFD-4512-AF89-1C2A09D9DCD3}" name="Table2" displayName="Table2" ref="A1:E32" totalsRowShown="0">
-  <autoFilter ref="A1:E32" xr:uid="{8040AE00-58DA-439D-815B-777F5227B716}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{04702736-6AFD-4512-AF89-1C2A09D9DCD3}" name="Table2" displayName="Table2" ref="A1:E33" totalsRowShown="0">
+  <autoFilter ref="A1:E33" xr:uid="{8040AE00-58DA-439D-815B-777F5227B716}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2D51013C-8C20-4AC9-B5B5-A03ABA0CC7AF}" name="Metric"/>
     <tableColumn id="2" xr3:uid="{C27B7664-1E3C-4879-8C79-28B1E9A1F763}" name="NEO-M8Q-01A"/>
@@ -877,8 +901,8 @@
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
@@ -1486,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50BCB51-82B5-48D2-BD5C-171740C85E68}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1497,7 +1521,7 @@
     <col min="1" max="1" width="21.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.1015625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.05078125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1547,6 +1571,9 @@
       <c r="D3" t="s">
         <v>112</v>
       </c>
+      <c r="E3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -1561,6 +1588,9 @@
       <c r="D4" t="s">
         <v>113</v>
       </c>
+      <c r="E4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -1575,11 +1605,26 @@
       <c r="D5" t="s">
         <v>114</v>
       </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -1599,6 +1644,9 @@
       <c r="D8" t="s">
         <v>86</v>
       </c>
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
@@ -1613,6 +1661,9 @@
       <c r="D9" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
@@ -1637,6 +1688,9 @@
       <c r="D12" t="s">
         <v>111</v>
       </c>
+      <c r="E12" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
@@ -1664,7 +1718,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -1677,8 +1731,11 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -1691,8 +1748,11 @@
       <c r="D18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -1705,8 +1765,11 @@
       <c r="D19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -1719,8 +1782,11 @@
       <c r="D20" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -1733,158 +1799,211 @@
       <c r="D21">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
         <v>90</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>119</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>119</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+      <c r="E23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
         <v>91</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>92</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>92</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
+      <c r="E24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
         <v>93</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>99</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>99</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
         <v>94</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>98</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
+      <c r="E26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
         <v>95</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>100</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>122</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+      <c r="E27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>96</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>101</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+      <c r="E28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
         <v>97</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>102</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>123</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
+      <c r="E30" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
+      <c r="E31" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
+      <c r="E32" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>